<commit_message>
changes in lls patient, pharmacy provider
</commit_message>
<xml_diff>
--- a/QA/testcases/LLS/Provider/L_Prov_Patient_App_Create_PCase_Positive.xlsx
+++ b/QA/testcases/LLS/Provider/L_Prov_Patient_App_Create_PCase_Positive.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27465" windowHeight="13650"/>
+    <workbookView windowWidth="28680" windowHeight="13650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -548,10 +548,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -583,6 +583,27 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -598,10 +619,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -613,24 +635,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -645,28 +690,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -674,34 +697,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -720,8 +719,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -754,187 +754,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1007,6 +1007,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1022,32 +1037,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1069,15 +1072,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1087,18 +1081,24 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1116,130 +1116,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1645,7 +1645,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:A33"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -1715,7 +1715,7 @@
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
lls time and poe2 prov
</commit_message>
<xml_diff>
--- a/QA/testcases/LLS/Provider/L_Prov_Patient_App_Create_PCase_Positive.xlsx
+++ b/QA/testcases/LLS/Provider/L_Prov_Patient_App_Create_PCase_Positive.xlsx
@@ -549,9 +549,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -584,23 +584,32 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -619,11 +628,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -636,28 +644,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -689,14 +675,37 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -711,17 +720,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -754,19 +754,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -778,25 +838,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -808,133 +928,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -998,6 +998,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1037,24 +1061,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1081,24 +1087,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1116,130 +1116,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1644,8 +1644,8 @@
   <sheetPr/>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -1781,7 +1781,7 @@
       <c r="C6" s="12"/>
       <c r="D6" s="12"/>
       <c r="E6" s="12">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -1857,7 +1857,7 @@
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="9">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>

</xml_diff>

<commit_message>
remiited poe 3 flows in lls phar and prov
</commit_message>
<xml_diff>
--- a/QA/testcases/LLS/Provider/L_Prov_Patient_App_Create_PCase_Positive.xlsx
+++ b/QA/testcases/LLS/Provider/L_Prov_Patient_App_Create_PCase_Positive.xlsx
@@ -548,10 +548,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -583,33 +583,11 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -622,14 +600,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -652,24 +655,51 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -684,29 +714,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -714,14 +721,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -754,31 +754,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -790,151 +922,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -998,30 +998,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1032,16 +1008,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1062,16 +1038,40 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1098,7 +1098,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1116,130 +1116,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1644,8 +1644,8 @@
   <sheetPr/>
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15" outlineLevelCol="7"/>

</xml_diff>